<commit_message>
fix to g_a_v_c_excel. Applied at the beginning of Cluster_Fucking. And the excel files from g_a_v_c_excel.
</commit_message>
<xml_diff>
--- a/May_17_Delivery_Data.xlsx
+++ b/May_17_Delivery_Data.xlsx
@@ -15,15 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="471">
   <si>
     <t>Facility Name</t>
   </si>
   <si>
-    <t>Facility Latitude</t>
-  </si>
-  <si>
-    <t>Facility Longitude</t>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
   <si>
     <t>Deliv Center Capac</t>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>Delivery Volume</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
   </si>
   <si>
     <t>640 6TH HOUSTON, TX, 77007</t>
@@ -1883,10 +1877,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1894,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1911,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1928,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1945,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1962,7 +1956,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1979,7 +1973,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1996,7 +1990,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2013,7 +2007,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2030,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>39</v>
@@ -2047,7 +2041,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2064,7 +2058,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2081,7 +2075,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2098,7 +2092,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2115,7 +2109,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2132,7 +2126,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2149,7 +2143,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -2166,7 +2160,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2183,7 +2177,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -2200,7 +2194,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -2217,7 +2211,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -2234,7 +2228,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -2251,7 +2245,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2268,7 +2262,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2285,7 +2279,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2302,7 +2296,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -2319,7 +2313,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2336,7 +2330,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2353,7 +2347,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -2370,7 +2364,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2387,7 +2381,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2404,7 +2398,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2421,7 +2415,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2438,7 +2432,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2455,7 +2449,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2472,7 +2466,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2489,7 +2483,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -2506,7 +2500,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2523,7 +2517,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2540,7 +2534,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2557,7 +2551,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2574,7 +2568,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>56</v>
@@ -2591,7 +2585,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2608,7 +2602,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2625,7 +2619,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2642,7 +2636,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2659,7 +2653,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -2676,7 +2670,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2693,7 +2687,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C49">
         <v>13</v>
@@ -2710,7 +2704,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2727,7 +2721,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2744,7 +2738,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2761,7 +2755,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2778,7 +2772,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2795,7 +2789,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2812,7 +2806,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2829,7 +2823,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -2846,7 +2840,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2863,7 +2857,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2880,7 +2874,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2897,7 +2891,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2914,7 +2908,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2931,7 +2925,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -2948,7 +2942,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -2965,7 +2959,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -2982,7 +2976,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2999,7 +2993,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -3016,7 +3010,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3033,7 +3027,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3050,7 +3044,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -3067,7 +3061,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -3084,7 +3078,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -3101,7 +3095,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -3118,7 +3112,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -3135,7 +3129,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -3152,7 +3146,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -3169,7 +3163,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -3186,7 +3180,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C78">
         <v>11</v>
@@ -3203,7 +3197,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C79">
         <v>7</v>
@@ -3220,7 +3214,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3237,7 +3231,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3254,7 +3248,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3271,7 +3265,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3288,7 +3282,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -3305,7 +3299,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -3322,7 +3316,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -3339,7 +3333,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -3356,7 +3350,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C88">
         <v>6</v>
@@ -3373,7 +3367,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -3390,7 +3384,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C90">
         <v>2</v>
@@ -3407,7 +3401,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -3424,7 +3418,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -3441,7 +3435,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -3458,7 +3452,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -3475,7 +3469,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -3492,7 +3486,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C96">
         <v>2</v>
@@ -3509,7 +3503,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C97">
         <v>2</v>
@@ -3526,7 +3520,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C98">
         <v>2</v>
@@ -3543,7 +3537,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C99">
         <v>4</v>
@@ -3560,7 +3554,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -3577,7 +3571,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -3594,7 +3588,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C102">
         <v>2</v>
@@ -3611,7 +3605,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -3628,7 +3622,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C104">
         <v>2</v>
@@ -3645,7 +3639,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -3662,7 +3656,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -3679,7 +3673,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C107">
         <v>4</v>
@@ -3696,7 +3690,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C108">
         <v>2</v>
@@ -3713,7 +3707,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -3730,7 +3724,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C110">
         <v>2</v>
@@ -3747,7 +3741,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C111">
         <v>3</v>
@@ -3764,7 +3758,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C112">
         <v>2</v>
@@ -3781,7 +3775,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C113">
         <v>5</v>
@@ -3798,7 +3792,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -3815,7 +3809,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -3832,7 +3826,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -3849,7 +3843,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -3866,7 +3860,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -3883,7 +3877,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -3900,7 +3894,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -3917,7 +3911,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -3934,7 +3928,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -3951,7 +3945,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3968,7 +3962,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C124">
         <v>2</v>
@@ -3985,7 +3979,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C125">
         <v>2</v>
@@ -4002,7 +3996,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -4019,7 +4013,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -4036,7 +4030,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -4053,7 +4047,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C129">
         <v>2</v>
@@ -4070,7 +4064,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -4087,7 +4081,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -4104,7 +4098,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -4121,7 +4115,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C133">
         <v>2</v>
@@ -4138,7 +4132,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C134">
         <v>9</v>
@@ -4155,7 +4149,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -4172,7 +4166,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -4189,7 +4183,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C137">
         <v>2</v>
@@ -4206,7 +4200,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C138">
         <v>27</v>
@@ -4223,7 +4217,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C139">
         <v>4</v>
@@ -4240,7 +4234,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -4257,7 +4251,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -4274,7 +4268,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -4291,7 +4285,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -4308,7 +4302,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -4325,7 +4319,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -4342,7 +4336,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -4359,7 +4353,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C147">
         <v>2</v>
@@ -4376,7 +4370,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -4393,7 +4387,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C149">
         <v>8</v>
@@ -4410,7 +4404,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -4427,7 +4421,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C151">
         <v>3</v>
@@ -4444,7 +4438,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -4461,7 +4455,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -4478,7 +4472,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -4495,7 +4489,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C155">
         <v>5</v>
@@ -4512,7 +4506,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -4529,7 +4523,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -4546,7 +4540,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -4563,7 +4557,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -4580,7 +4574,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -4597,7 +4591,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -4614,7 +4608,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C162">
         <v>2</v>
@@ -4631,7 +4625,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -4648,7 +4642,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -4665,7 +4659,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -4682,7 +4676,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -4699,7 +4693,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -4716,7 +4710,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C168">
         <v>1</v>
@@ -4733,7 +4727,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -4750,7 +4744,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -4767,7 +4761,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -4784,7 +4778,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C172">
         <v>2</v>
@@ -4801,7 +4795,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -4818,7 +4812,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C174">
         <v>2</v>
@@ -4835,7 +4829,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C175">
         <v>6</v>
@@ -4852,7 +4846,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C176">
         <v>2</v>
@@ -4869,7 +4863,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C177">
         <v>2</v>
@@ -4886,7 +4880,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C178">
         <v>2</v>
@@ -4903,7 +4897,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -4920,7 +4914,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -4937,7 +4931,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -4954,7 +4948,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -4971,7 +4965,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -4988,7 +4982,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -5005,7 +4999,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -5022,7 +5016,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -5039,7 +5033,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -5056,7 +5050,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C188">
         <v>3</v>
@@ -5073,7 +5067,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C189">
         <v>2</v>
@@ -5090,7 +5084,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -5107,7 +5101,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -5124,7 +5118,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C192">
         <v>2</v>
@@ -5141,7 +5135,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -5158,7 +5152,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -5175,7 +5169,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -5192,7 +5186,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C196">
         <v>2</v>
@@ -5209,7 +5203,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -5226,7 +5220,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -5243,7 +5237,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -5260,7 +5254,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -5277,7 +5271,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -5294,7 +5288,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -5311,7 +5305,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C203">
         <v>1</v>
@@ -5328,7 +5322,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -5345,7 +5339,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -5362,7 +5356,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -5379,7 +5373,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -5396,7 +5390,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -5413,7 +5407,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C209">
         <v>3</v>
@@ -5430,7 +5424,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -5447,7 +5441,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -5464,7 +5458,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C212">
         <v>5</v>
@@ -5481,7 +5475,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C213">
         <v>2</v>
@@ -5498,7 +5492,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C214">
         <v>1</v>
@@ -5515,7 +5509,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -5532,7 +5526,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -5549,7 +5543,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C217">
         <v>2</v>
@@ -5566,7 +5560,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C218">
         <v>1</v>
@@ -5583,7 +5577,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -5600,7 +5594,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -5617,7 +5611,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -5634,7 +5628,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -5651,7 +5645,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -5668,7 +5662,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -5685,7 +5679,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -5702,7 +5696,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C226">
         <v>2</v>
@@ -5719,7 +5713,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C227">
         <v>2</v>
@@ -5736,7 +5730,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -5753,7 +5747,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -5770,7 +5764,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -5787,7 +5781,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -5804,7 +5798,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C232">
         <v>8</v>
@@ -5821,7 +5815,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -5838,7 +5832,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C234">
         <v>1</v>
@@ -5855,7 +5849,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C235">
         <v>2</v>
@@ -5872,7 +5866,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C236">
         <v>1</v>
@@ -5889,7 +5883,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C237">
         <v>3</v>
@@ -5906,7 +5900,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C238">
         <v>1</v>
@@ -5923,7 +5917,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -5940,7 +5934,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C240">
         <v>1</v>
@@ -5957,7 +5951,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C241">
         <v>1</v>
@@ -5974,7 +5968,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C242">
         <v>1</v>
@@ -5991,7 +5985,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -6008,7 +6002,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -6025,7 +6019,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C245">
         <v>2</v>
@@ -6042,7 +6036,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C246">
         <v>2</v>
@@ -6059,7 +6053,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -6076,7 +6070,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -6093,7 +6087,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -6110,7 +6104,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -6127,7 +6121,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -6144,7 +6138,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -6161,7 +6155,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -6178,7 +6172,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -6195,7 +6189,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C255">
         <v>2</v>
@@ -6212,7 +6206,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C256">
         <v>2</v>
@@ -6229,7 +6223,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -6246,7 +6240,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -6263,7 +6257,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -6280,7 +6274,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C260">
         <v>3</v>
@@ -6297,7 +6291,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -6314,7 +6308,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C262">
         <v>1</v>
@@ -6331,7 +6325,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C263">
         <v>1</v>
@@ -6348,7 +6342,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C264">
         <v>1</v>
@@ -6365,7 +6359,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C265">
         <v>2</v>
@@ -6382,7 +6376,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -6399,7 +6393,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C267">
         <v>2</v>
@@ -6416,7 +6410,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C268">
         <v>4</v>
@@ -6433,7 +6427,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -6450,7 +6444,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C270">
         <v>2</v>
@@ -6467,7 +6461,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C271">
         <v>1</v>
@@ -6484,7 +6478,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -6501,7 +6495,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C273">
         <v>4</v>
@@ -6518,7 +6512,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C274">
         <v>1</v>
@@ -6535,7 +6529,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C275">
         <v>1</v>
@@ -6552,7 +6546,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C276">
         <v>1</v>
@@ -6569,7 +6563,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C277">
         <v>1</v>
@@ -6586,7 +6580,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C278">
         <v>1</v>
@@ -6603,7 +6597,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C279">
         <v>1</v>
@@ -6620,7 +6614,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C280">
         <v>1</v>
@@ -6637,7 +6631,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C281">
         <v>1</v>
@@ -6654,7 +6648,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C282">
         <v>1</v>
@@ -6671,7 +6665,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C283">
         <v>1</v>
@@ -6688,7 +6682,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C284">
         <v>1</v>
@@ -6705,7 +6699,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C285">
         <v>1</v>
@@ -6722,7 +6716,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C286">
         <v>2</v>
@@ -6739,7 +6733,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C287">
         <v>1</v>
@@ -6756,7 +6750,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C288">
         <v>1</v>
@@ -6773,7 +6767,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -6790,7 +6784,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C290">
         <v>1</v>
@@ -6807,7 +6801,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C291">
         <v>1</v>
@@ -6824,7 +6818,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C292">
         <v>3</v>
@@ -6841,7 +6835,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -6858,7 +6852,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C294">
         <v>1</v>
@@ -6875,7 +6869,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C295">
         <v>3</v>
@@ -6892,7 +6886,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C296">
         <v>1</v>
@@ -6909,7 +6903,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C297">
         <v>3</v>
@@ -6926,7 +6920,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C298">
         <v>2</v>
@@ -6943,7 +6937,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C299">
         <v>1</v>
@@ -6960,7 +6954,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C300">
         <v>2</v>
@@ -6977,7 +6971,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C301">
         <v>1</v>
@@ -6994,7 +6988,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C302">
         <v>1</v>
@@ -7011,7 +7005,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C303">
         <v>2</v>
@@ -7028,7 +7022,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C304">
         <v>1</v>
@@ -7045,7 +7039,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C305">
         <v>1</v>
@@ -7062,7 +7056,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C306">
         <v>2</v>
@@ -7079,7 +7073,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C307">
         <v>4</v>
@@ -7096,7 +7090,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C308">
         <v>5</v>
@@ -7113,7 +7107,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C309">
         <v>1</v>
@@ -7130,7 +7124,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C310">
         <v>1</v>
@@ -7147,7 +7141,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C311">
         <v>2</v>
@@ -7164,7 +7158,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C312">
         <v>1</v>
@@ -7181,7 +7175,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C313">
         <v>2</v>
@@ -7198,7 +7192,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C314">
         <v>1</v>
@@ -7215,7 +7209,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C315">
         <v>1</v>
@@ -7232,7 +7226,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C316">
         <v>1</v>
@@ -7249,7 +7243,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C317">
         <v>2</v>
@@ -7266,7 +7260,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C318">
         <v>4</v>
@@ -7283,7 +7277,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C319">
         <v>8</v>
@@ -7300,7 +7294,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C320">
         <v>1</v>
@@ -7317,7 +7311,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C321">
         <v>1</v>
@@ -7334,7 +7328,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C322">
         <v>1</v>
@@ -7351,7 +7345,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C323">
         <v>1</v>
@@ -7368,7 +7362,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C324">
         <v>4</v>
@@ -7385,7 +7379,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C325">
         <v>1</v>
@@ -7402,7 +7396,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C326">
         <v>1</v>
@@ -7419,7 +7413,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C327">
         <v>1</v>
@@ -7436,7 +7430,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C328">
         <v>1</v>
@@ -7453,7 +7447,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C329">
         <v>1</v>
@@ -7470,7 +7464,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C330">
         <v>1</v>
@@ -7487,7 +7481,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C331">
         <v>1</v>
@@ -7504,7 +7498,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C332">
         <v>1</v>
@@ -7521,7 +7515,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C333">
         <v>1</v>
@@ -7538,7 +7532,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C334">
         <v>6</v>
@@ -7555,7 +7549,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C335">
         <v>2</v>
@@ -7572,7 +7566,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C336">
         <v>1</v>
@@ -7589,7 +7583,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C337">
         <v>1</v>
@@ -7606,7 +7600,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C338">
         <v>4</v>
@@ -7623,7 +7617,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C339">
         <v>1</v>
@@ -7640,7 +7634,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C340">
         <v>3</v>
@@ -7657,7 +7651,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C341">
         <v>2</v>
@@ -7674,7 +7668,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C342">
         <v>2</v>
@@ -7691,7 +7685,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C343">
         <v>1</v>
@@ -7708,7 +7702,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C344">
         <v>1</v>
@@ -7725,7 +7719,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C345">
         <v>1</v>
@@ -7742,7 +7736,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C346">
         <v>2</v>
@@ -7759,7 +7753,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C347">
         <v>1</v>
@@ -7776,7 +7770,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C348">
         <v>3</v>
@@ -7793,7 +7787,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C349">
         <v>1</v>
@@ -7810,7 +7804,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C350">
         <v>1</v>
@@ -7827,7 +7821,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C351">
         <v>1</v>
@@ -7844,7 +7838,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C352">
         <v>1</v>
@@ -7861,7 +7855,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C353">
         <v>1</v>
@@ -7878,7 +7872,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C354">
         <v>1</v>
@@ -7895,7 +7889,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C355">
         <v>1</v>
@@ -7912,7 +7906,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C356">
         <v>1</v>
@@ -7929,7 +7923,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C357">
         <v>1</v>
@@ -7946,7 +7940,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C358">
         <v>1</v>
@@ -7963,7 +7957,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C359">
         <v>2</v>
@@ -7980,7 +7974,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C360">
         <v>1</v>
@@ -7997,7 +7991,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C361">
         <v>1</v>
@@ -8014,7 +8008,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C362">
         <v>1</v>
@@ -8031,7 +8025,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C363">
         <v>1</v>
@@ -8048,7 +8042,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C364">
         <v>1</v>
@@ -8065,7 +8059,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C365">
         <v>1</v>
@@ -8082,7 +8076,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C366">
         <v>1</v>
@@ -8099,7 +8093,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C367">
         <v>1</v>
@@ -8116,7 +8110,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C368">
         <v>2</v>
@@ -8133,7 +8127,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C369">
         <v>1</v>
@@ -8150,7 +8144,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C370">
         <v>1</v>
@@ -8167,7 +8161,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C371">
         <v>2</v>
@@ -8184,7 +8178,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C372">
         <v>1</v>
@@ -8201,7 +8195,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C373">
         <v>1</v>
@@ -8218,7 +8212,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C374">
         <v>2</v>
@@ -8235,7 +8229,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C375">
         <v>1</v>
@@ -8252,7 +8246,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C376">
         <v>2</v>
@@ -8269,7 +8263,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C377">
         <v>1</v>
@@ -8286,7 +8280,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C378">
         <v>2</v>
@@ -8303,7 +8297,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C379">
         <v>2</v>
@@ -8320,7 +8314,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C380">
         <v>1</v>
@@ -8337,7 +8331,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C381">
         <v>1</v>
@@ -8354,7 +8348,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C382">
         <v>1</v>
@@ -8371,7 +8365,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C383">
         <v>1</v>
@@ -8388,7 +8382,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C384">
         <v>1</v>
@@ -8405,7 +8399,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C385">
         <v>2</v>
@@ -8422,7 +8416,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C386">
         <v>1</v>
@@ -8439,7 +8433,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C387">
         <v>1</v>
@@ -8456,7 +8450,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C388">
         <v>1</v>
@@ -8473,7 +8467,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C389">
         <v>1</v>
@@ -8490,7 +8484,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C390">
         <v>1</v>
@@ -8507,7 +8501,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C391">
         <v>1</v>
@@ -8524,7 +8518,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C392">
         <v>1</v>
@@ -8541,7 +8535,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C393">
         <v>2</v>
@@ -8558,7 +8552,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C394">
         <v>1</v>
@@ -8575,7 +8569,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C395">
         <v>1</v>
@@ -8592,7 +8586,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C396">
         <v>2</v>
@@ -8609,7 +8603,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C397">
         <v>2</v>
@@ -8626,7 +8620,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C398">
         <v>2</v>
@@ -8643,7 +8637,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C399">
         <v>1</v>
@@ -8660,7 +8654,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C400">
         <v>1</v>
@@ -8677,7 +8671,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C401">
         <v>1</v>
@@ -8694,7 +8688,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C402">
         <v>1</v>
@@ -8711,7 +8705,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C403">
         <v>1</v>
@@ -8728,7 +8722,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -8745,7 +8739,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -8762,7 +8756,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C406">
         <v>1</v>
@@ -8779,7 +8773,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C407">
         <v>1</v>
@@ -8796,7 +8790,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C408">
         <v>1</v>
@@ -8813,7 +8807,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C409">
         <v>1</v>
@@ -8830,7 +8824,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C410">
         <v>1</v>
@@ -8847,7 +8841,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C411">
         <v>1</v>
@@ -8864,7 +8858,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C412">
         <v>1</v>
@@ -8881,7 +8875,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C413">
         <v>2</v>
@@ -8898,7 +8892,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C414">
         <v>1</v>
@@ -8915,7 +8909,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C415">
         <v>2</v>
@@ -8932,7 +8926,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C416">
         <v>1</v>
@@ -8949,7 +8943,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C417">
         <v>1</v>
@@ -8966,7 +8960,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C418">
         <v>1</v>
@@ -8983,7 +8977,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C419">
         <v>2</v>
@@ -9000,7 +8994,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C420">
         <v>1</v>
@@ -9017,7 +9011,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C421">
         <v>1</v>
@@ -9034,7 +9028,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -9051,7 +9045,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C423">
         <v>1</v>
@@ -9068,7 +9062,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C424">
         <v>2</v>
@@ -9085,7 +9079,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -9102,7 +9096,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C426">
         <v>4</v>
@@ -9119,7 +9113,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C427">
         <v>1</v>
@@ -9136,7 +9130,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C428">
         <v>4</v>
@@ -9153,7 +9147,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C429">
         <v>1</v>
@@ -9170,7 +9164,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C430">
         <v>1</v>
@@ -9187,7 +9181,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C431">
         <v>1</v>
@@ -9204,7 +9198,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C432">
         <v>1</v>
@@ -9221,7 +9215,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C433">
         <v>4</v>
@@ -9238,7 +9232,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C434">
         <v>2</v>
@@ -9255,7 +9249,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C435">
         <v>6</v>
@@ -9272,7 +9266,7 @@
         <v>434</v>
       </c>
       <c r="B436" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C436">
         <v>3</v>
@@ -9289,7 +9283,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C437">
         <v>2</v>
@@ -9306,7 +9300,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C438">
         <v>1</v>
@@ -9323,7 +9317,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C439">
         <v>1</v>
@@ -9340,7 +9334,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C440">
         <v>2</v>
@@ -9357,7 +9351,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C441">
         <v>4</v>
@@ -9374,7 +9368,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C442">
         <v>2</v>
@@ -9391,7 +9385,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C443">
         <v>1</v>
@@ -9408,7 +9402,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C444">
         <v>1</v>
@@ -9425,7 +9419,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C445">
         <v>2</v>
@@ -9442,7 +9436,7 @@
         <v>444</v>
       </c>
       <c r="B446" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C446">
         <v>1</v>
@@ -9459,7 +9453,7 @@
         <v>445</v>
       </c>
       <c r="B447" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C447">
         <v>3</v>
@@ -9476,7 +9470,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C448">
         <v>15</v>
@@ -9493,7 +9487,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C449">
         <v>1</v>
@@ -9510,7 +9504,7 @@
         <v>448</v>
       </c>
       <c r="B450" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C450">
         <v>1</v>
@@ -9527,7 +9521,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C451">
         <v>1</v>
@@ -9544,7 +9538,7 @@
         <v>450</v>
       </c>
       <c r="B452" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C452">
         <v>2</v>
@@ -9561,7 +9555,7 @@
         <v>451</v>
       </c>
       <c r="B453" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C453">
         <v>1</v>
@@ -9578,7 +9572,7 @@
         <v>452</v>
       </c>
       <c r="B454" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C454">
         <v>2</v>
@@ -9595,7 +9589,7 @@
         <v>453</v>
       </c>
       <c r="B455" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C455">
         <v>1</v>
@@ -9612,7 +9606,7 @@
         <v>454</v>
       </c>
       <c r="B456" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C456">
         <v>1</v>
@@ -9629,7 +9623,7 @@
         <v>455</v>
       </c>
       <c r="B457" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C457">
         <v>1</v>
@@ -9646,7 +9640,7 @@
         <v>456</v>
       </c>
       <c r="B458" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C458">
         <v>1</v>
@@ -9663,7 +9657,7 @@
         <v>457</v>
       </c>
       <c r="B459" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C459">
         <v>1</v>
@@ -9680,7 +9674,7 @@
         <v>458</v>
       </c>
       <c r="B460" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C460">
         <v>1</v>
@@ -9697,7 +9691,7 @@
         <v>459</v>
       </c>
       <c r="B461" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C461">
         <v>2</v>
@@ -9714,7 +9708,7 @@
         <v>460</v>
       </c>
       <c r="B462" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C462">
         <v>1</v>
@@ -9731,7 +9725,7 @@
         <v>461</v>
       </c>
       <c r="B463" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C463">
         <v>1</v>
@@ -9748,7 +9742,7 @@
         <v>462</v>
       </c>
       <c r="B464" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C464">
         <v>1</v>
@@ -9765,7 +9759,7 @@
         <v>463</v>
       </c>
       <c r="B465" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C465">
         <v>1</v>
@@ -9782,7 +9776,7 @@
         <v>464</v>
       </c>
       <c r="B466" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C466">
         <v>1</v>

</xml_diff>